<commit_message>
Range Excel Files Added
</commit_message>
<xml_diff>
--- a/Experiments_Code/Motion_Compensation_Experiment/Motion_Experiment_HighFilt.xlsx
+++ b/Experiments_Code/Motion_Compensation_Experiment/Motion_Experiment_HighFilt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamin\Desktop\LiDAR_Motion_Comp_Feature_Extract_Repo\LiDAR-Motion-Compensation-and-Feature-Extraction\Experiments_Code\Motion_Compensation_Experiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FD15CA-5D5A-40AA-9B34-681A892FCC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0862B572-B165-4B64-B2A6-E89FA5BE66F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{CFDFB1C6-CAB1-48A8-A21A-6A992CCE1E77}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{CFDFB1C6-CAB1-48A8-A21A-6A992CCE1E77}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5736,8 +5736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7340EEC-1106-4737-A1A6-7539F195561E}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>